<commit_message>
Bigfit bug squash and update
Fixed excel exporting overwriting bug
</commit_message>
<xml_diff>
--- a/big_fit/compiled_data.xlsx
+++ b/big_fit/compiled_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\ResearchHome\Groups\millergrp\home\common\Python\_pete\big_fit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8F565A-A159-4B23-8F13-840D2404AD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8C3561-EFFD-4B4B-BFAD-3FA6B9708BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="65">
   <si>
     <t>CAGE#</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Miller-Plate37-A03</t>
   </si>
   <si>
-    <t>d7</t>
-  </si>
-  <si>
     <t>Miller-Plate37-A04</t>
   </si>
   <si>
@@ -151,9 +148,6 @@
     <t>Miller-Plate37-A06</t>
   </si>
   <si>
-    <t>d21</t>
-  </si>
-  <si>
     <t>Miller-Plate37-A07</t>
   </si>
   <si>
@@ -227,6 +221,15 @@
   </si>
   <si>
     <t>d28.g9</t>
+  </si>
+  <si>
+    <t>d21.g46</t>
+  </si>
+  <si>
+    <t>d21.g9</t>
+  </si>
+  <si>
+    <t>d7.g9</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,8 +639,8 @@
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -687,7 +690,7 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2">
         <v>95.1</v>
@@ -713,7 +716,7 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3">
         <v>26.7</v>
@@ -725,7 +728,10 @@
         <v>59.2</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
+        <v>50</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
@@ -745,7 +751,7 @@
         <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="F4">
         <v>24.8</v>
@@ -754,7 +760,16 @@
         <v>12.2</v>
       </c>
       <c r="H4">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -765,13 +780,13 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F5">
         <v>25.2</v>
@@ -791,13 +806,13 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6">
         <v>26.9</v>
@@ -817,13 +832,13 @@
         <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="F7">
         <v>35.1</v>
@@ -833,6 +848,15 @@
       </c>
       <c r="H7">
         <v>52.5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -843,13 +867,13 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8">
         <v>30.5</v>
@@ -861,7 +885,10 @@
         <v>58</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
       </c>
       <c r="K8" t="s">
         <v>17</v>
@@ -872,16 +899,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F9">
         <v>99.6</v>
@@ -898,16 +925,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>42</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F10">
         <v>94</v>
@@ -919,10 +946,13 @@
         <v>4.3</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="J10" t="s">
+        <v>53</v>
       </c>
       <c r="K10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -930,16 +960,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
         <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="F11">
         <v>92.9</v>
@@ -949,6 +979,15 @@
       </c>
       <c r="H11">
         <v>5.4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -956,16 +995,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
         <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12">
         <v>94.5</v>
@@ -982,16 +1021,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13">
         <v>92.6</v>
@@ -1008,16 +1047,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
         <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>95.1</v>
@@ -1027,6 +1066,15 @@
       </c>
       <c r="H14">
         <v>4.2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>49</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1034,16 +1082,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
         <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F15">
         <v>96.3</v>
@@ -1055,10 +1103,13 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>53</v>
       </c>
       <c r="K15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4610,10 +4661,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -4624,10 +4675,10 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I3" t="s">
         <v>13</v>
@@ -4638,10 +4689,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
@@ -4652,10 +4703,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
         <v>21</v>
@@ -4663,7 +4714,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -4671,7 +4722,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>

</xml_diff>